<commit_message>
Fix minor issues in new documentation page. Change TDC metadata parsing logic to better align with other handling of '#ignore'
</commit_message>
<xml_diff>
--- a/tests/sir_databook_comment_test.xlsx
+++ b/tests/sir_databook_comment_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26085BE1-3C02-46F8-A823-E8723623F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DBDB14-3FA9-4E1E-B854-C26D5AE937D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="1785" windowWidth="32385" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7590" yWindow="2550" windowWidth="32385" windowHeight="15690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="46">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>This row will be treated as a blank row, and can separate the two TDVE tables</t>
+  </si>
+  <si>
+    <t>Extra attribute</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -301,7 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,9 +326,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
@@ -340,31 +343,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
+  <dxfs count="70">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -462,6 +441,18 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor rgb="FF98E0FA"/>
         </patternFill>
@@ -477,6 +468,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF98E0FA"/>
         </patternFill>
       </fill>
@@ -492,83 +490,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98E0FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA500"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1020,6 +941,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98E0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98E0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98E0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98E0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98E0FA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1454,7 +1445,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1531,8 +1522,8 @@
   </sheetPr>
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1535,7 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1561,12 +1552,13 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="9"/>
       <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1583,47 +1575,47 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="str">
@@ -1642,8 +1634,8 @@
         <f>'Population Definitions'!$A$5</f>
         <v>Adults 65+</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1664,10 +1656,10 @@
       <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1688,10 +1680,10 @@
       <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1712,10 +1704,10 @@
       <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1736,31 +1728,31 @@
       <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1998,7 +1990,7 @@
       <c r="M28" s="1">
         <v>2007</v>
       </c>
-      <c r="N28" s="7"/>
+      <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
@@ -2021,16 +2013,16 @@
         <v>...</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="K29" s="7">
+      <c r="K29" s="4">
         <v>0.53268194497174115</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="4">
         <v>0.70070831689130797</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="4">
         <v>0.82467874024093191</v>
       </c>
-      <c r="N29" s="7"/>
+      <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
@@ -2053,16 +2045,16 @@
         <v>...</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="K30" s="7">
+      <c r="K30" s="4">
         <v>2.7957843186858011E-2</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="4">
         <v>0.73377203891453735</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30" s="4">
         <v>7.0670376076250485E-2</v>
       </c>
-      <c r="N30" s="7"/>
+      <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
@@ -2087,16 +2079,16 @@
         <v>OR</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="K31" s="7">
+      <c r="K31" s="4">
         <v>0.80337364762719154</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="4">
         <v>0.48004592967418935</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="4">
         <v>0.26208156403516669</v>
       </c>
-      <c r="N31" s="7"/>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
@@ -2588,255 +2580,257 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:B10">
-    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="45" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="46" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="cellIs" dxfId="69" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="117" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="118" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B51:B53">
+    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="12" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="67" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="40" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C10">
-    <cfRule type="cellIs" dxfId="65" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="53" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="63" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="111" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="112" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="cellIs" dxfId="61" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="125" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="126" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C53">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="14" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="cellIs" dxfId="59" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="42" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="41" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="42" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="62" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="47" priority="113" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="114" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="55" priority="113" operator="equal">
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" dxfId="45" priority="133" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="134" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="53" priority="133" operator="equal">
+  <conditionalFormatting sqref="D50:D51">
+    <cfRule type="cellIs" dxfId="43" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D15:H15">
-    <cfRule type="expression" dxfId="51" priority="65">
+    <cfRule type="expression" dxfId="39" priority="65">
       <formula>$B$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:H16">
-    <cfRule type="expression" dxfId="50" priority="68">
+    <cfRule type="expression" dxfId="38" priority="68">
       <formula>$C$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:I17">
-    <cfRule type="expression" dxfId="49" priority="71">
+    <cfRule type="expression" dxfId="37" priority="71">
       <formula>$D$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:I29">
-    <cfRule type="expression" dxfId="48" priority="137">
+    <cfRule type="expression" dxfId="36" priority="137">
       <formula>$B$23&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:I30">
-    <cfRule type="expression" dxfId="47" priority="140">
+    <cfRule type="expression" dxfId="35" priority="140">
       <formula>$C$23&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:H56 D31:I31">
-    <cfRule type="expression" dxfId="46" priority="143">
+  <conditionalFormatting sqref="D31:I31 D56:H56">
+    <cfRule type="expression" dxfId="34" priority="143">
       <formula>$D$23&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:I32 D57:I57">
-    <cfRule type="expression" dxfId="45" priority="146">
+    <cfRule type="expression" dxfId="33" priority="146">
       <formula>$E$23&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:I33 D58:I58">
-    <cfRule type="expression" dxfId="44" priority="149">
+    <cfRule type="expression" dxfId="32" priority="149">
       <formula>$B$24&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:I34">
-    <cfRule type="expression" dxfId="43" priority="152">
+    <cfRule type="expression" dxfId="31" priority="152">
       <formula>$C$24&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:I35">
-    <cfRule type="expression" dxfId="42" priority="155">
+    <cfRule type="expression" dxfId="30" priority="155">
       <formula>$D$24&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:I36">
-    <cfRule type="expression" dxfId="41" priority="158">
+    <cfRule type="expression" dxfId="29" priority="158">
       <formula>$E$24&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:I37">
-    <cfRule type="expression" dxfId="40" priority="161">
+    <cfRule type="expression" dxfId="28" priority="161">
       <formula>$B$25&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:I38">
-    <cfRule type="expression" dxfId="39" priority="164">
+    <cfRule type="expression" dxfId="27" priority="164">
       <formula>$C$25&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:I39">
-    <cfRule type="expression" dxfId="38" priority="167">
+    <cfRule type="expression" dxfId="26" priority="167">
       <formula>$D$25&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:I40">
-    <cfRule type="expression" dxfId="37" priority="170">
+    <cfRule type="expression" dxfId="25" priority="170">
       <formula>$E$25&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41:I41">
-    <cfRule type="expression" dxfId="36" priority="173">
+    <cfRule type="expression" dxfId="24" priority="173">
       <formula>$B$26&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:I42">
-    <cfRule type="expression" dxfId="35" priority="176">
+    <cfRule type="expression" dxfId="23" priority="176">
       <formula>$C$26&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:I43">
-    <cfRule type="expression" dxfId="34" priority="179">
+    <cfRule type="expression" dxfId="22" priority="179">
       <formula>$D$26&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:I44">
-    <cfRule type="expression" dxfId="33" priority="182">
+    <cfRule type="expression" dxfId="21" priority="182">
       <formula>$E$26&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E9">
-    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="44" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="43" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="44" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E25">
+    <cfRule type="cellIs" dxfId="18" priority="116" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E25">
-    <cfRule type="cellIs" dxfId="30" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="115" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="116" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E52">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:B53">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52:C53">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50:D51">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E52">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
-      <formula>"N"</formula>
+  <conditionalFormatting sqref="G17 G29:G44 G57:G58">
+    <cfRule type="expression" dxfId="14" priority="246">
+      <formula>COUNTIF(I17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29:G44 G57:G58 G17">
+    <cfRule type="expression" dxfId="13" priority="247">
+      <formula>AND(COUNTIF(I17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(G17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>$C$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29:G44 G57:G58 G17">
-    <cfRule type="expression" dxfId="15" priority="246">
-      <formula>COUNTIF(I17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="247">
-      <formula>AND(COUNTIF(I17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(G17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2963,10 +2957,10 @@
       <c r="L1" s="1">
         <v>2005</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10">
+      <c r="N1" s="9">
         <v>2006</v>
       </c>
     </row>
@@ -2978,7 +2972,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="2">
@@ -2999,10 +2993,10 @@
       <c r="L2" s="2">
         <v>6</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3014,7 +3008,7 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="2"/>
@@ -3023,57 +3017,57 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="M3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="11"/>
+      <c r="B4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
@@ -3083,7 +3077,7 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="2"/>
@@ -3092,10 +3086,10 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="11" t="s">
+      <c r="M5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3107,7 +3101,7 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="2"/>
@@ -3116,42 +3110,42 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="M6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -3191,7 +3185,7 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="3"/>
@@ -3200,7 +3194,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3212,7 +3206,7 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="3"/>
@@ -3221,7 +3215,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3233,7 +3227,7 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="3"/>
@@ -3242,7 +3236,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3254,7 +3248,7 @@
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="3"/>
@@ -3263,71 +3257,71 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="11" t="s">
+      <c r="B13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="11" t="s">
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3606,10 +3600,10 @@
       <c r="G7" s="1">
         <v>2000</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J7" s="1"/>
@@ -3630,13 +3624,13 @@
       <c r="E8" s="3">
         <v>80</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="F8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J8" s="3"/>
@@ -3657,13 +3651,13 @@
       <c r="E9" s="3">
         <v>80</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="F9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J9" s="3"/>
@@ -3684,14 +3678,14 @@
       <c r="E10" s="3">
         <v>80</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="H10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J10" s="3"/>
@@ -3712,14 +3706,14 @@
       <c r="E11" s="3">
         <v>80</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="H11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J11" s="3"/>
@@ -4162,43 +4156,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E5 E10:E11">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>AND(COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E9">
+    <cfRule type="expression" dxfId="9" priority="254">
+      <formula>COUNTIF(H8:K8,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="255">
+      <formula>AND(COUNTIF(H8:K8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="6" priority="22">
       <formula>AND(COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E23">
-    <cfRule type="expression" dxfId="9" priority="29">
+    <cfRule type="expression" dxfId="5" priority="29">
       <formula>COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="30">
+    <cfRule type="expression" dxfId="4" priority="30">
       <formula>AND(COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E29">
-    <cfRule type="expression" dxfId="7" priority="37">
+    <cfRule type="expression" dxfId="3" priority="37">
       <formula>COUNTIF(G26:K26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="38">
+    <cfRule type="expression" dxfId="2" priority="38">
       <formula>AND(COUNTIF(G26:K26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E9">
-    <cfRule type="expression" dxfId="5" priority="254">
-      <formula>COUNTIF(H8:K8,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="255">
-      <formula>AND(COUNTIF(H8:K8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">

</xml_diff>